<commit_message>
web element definitions spreadsheet
</commit_message>
<xml_diff>
--- a/webelementdefinitions.xlsx
+++ b/webelementdefinitions.xlsx
@@ -12,7 +12,10 @@
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="global" sheetId="1" r:id="rId1"/>
+    <sheet name="BPTEventPage" sheetId="2" r:id="rId2"/>
+    <sheet name="BPTFindAnEventPage" sheetId="3" r:id="rId3"/>
+    <sheet name="BPTPaymentPage" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>//td[contains(text(),'Contact us')]</t>
   </si>
@@ -63,19 +66,30 @@
   </si>
   <si>
     <t>Event Producers</t>
+  </si>
+  <si>
+    <t>//img[contains(@src,'BPT_logo_drop_small.png')]</t>
+  </si>
+  <si>
+    <t>BPT_logo_drop_small.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Menlo"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,8 +112,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,16 +392,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C7"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -461,7 +477,55 @@
         <v>//td[contains(text(),'Event Producers')]</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="str">
+        <f>"//img[contains(@src,'"&amp;B12&amp;"')]"</f>
+        <v>//img[contains(@src,'BPT_logo_drop_small.png')]</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>